<commit_message>
[FIX] JUN double data
</commit_message>
<xml_diff>
--- a/data/AAT_Fluo_Data.xlsx
+++ b/data/AAT_Fluo_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="9" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="7" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="AlexaFluor350" sheetId="2" r:id="rId1"/>
@@ -54468,8 +54468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="F167" sqref="F167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56753,332 +56753,168 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="2">
-        <v>540</v>
-      </c>
-      <c r="B154" s="2">
-        <v>49.5</v>
-      </c>
+      <c r="A154" s="2"/>
+      <c r="B154" s="2"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="2">
-        <v>541</v>
-      </c>
-      <c r="B155" s="2">
-        <v>51</v>
-      </c>
+      <c r="A155" s="2"/>
+      <c r="B155" s="2"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A156" s="2">
-        <v>542</v>
-      </c>
-      <c r="B156" s="2">
-        <v>55</v>
-      </c>
+      <c r="A156" s="2"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A157" s="2">
-        <v>544</v>
-      </c>
-      <c r="B157" s="2">
-        <v>56.5</v>
-      </c>
+      <c r="A157" s="2"/>
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A158" s="2">
-        <v>545</v>
-      </c>
-      <c r="B158" s="2">
-        <v>59</v>
-      </c>
+      <c r="A158" s="2"/>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="2">
-        <v>547</v>
-      </c>
-      <c r="B159" s="2">
-        <v>64</v>
-      </c>
+      <c r="A159" s="2"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="2">
-        <v>548</v>
-      </c>
-      <c r="B160" s="2">
-        <v>67</v>
-      </c>
+      <c r="A160" s="2"/>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="2">
-        <v>550</v>
-      </c>
-      <c r="B161" s="2">
-        <v>73.5</v>
-      </c>
+      <c r="A161" s="2"/>
+      <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="2">
-        <v>551</v>
-      </c>
-      <c r="B162" s="2">
-        <v>77.5</v>
-      </c>
+      <c r="A162" s="2"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" s="2">
-        <v>552</v>
-      </c>
-      <c r="B163" s="2">
-        <v>81</v>
-      </c>
+      <c r="A163" s="2"/>
+      <c r="B163" s="2"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="2">
-        <v>553</v>
-      </c>
-      <c r="B164" s="2">
-        <v>88.5</v>
-      </c>
+      <c r="A164" s="2"/>
+      <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="2">
-        <v>555</v>
-      </c>
-      <c r="B165" s="2">
-        <v>91.5</v>
-      </c>
+      <c r="A165" s="2"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="2">
-        <v>556</v>
-      </c>
-      <c r="B166" s="2">
-        <v>94</v>
-      </c>
+      <c r="A166" s="2"/>
+      <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" s="2">
-        <v>557</v>
-      </c>
-      <c r="B167" s="2">
-        <v>97</v>
-      </c>
+      <c r="A167" s="2"/>
+      <c r="B167" s="2"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" s="2">
-        <v>558</v>
-      </c>
-      <c r="B168" s="2">
-        <v>100</v>
-      </c>
+      <c r="A168" s="2"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" s="2">
-        <v>560</v>
-      </c>
-      <c r="B169" s="2">
-        <v>100</v>
-      </c>
+      <c r="A169" s="2"/>
+      <c r="B169" s="2"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" s="2">
-        <v>561</v>
-      </c>
-      <c r="B170" s="2">
-        <v>100</v>
-      </c>
+      <c r="A170" s="2"/>
+      <c r="B170" s="2"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" s="2">
-        <v>562</v>
-      </c>
-      <c r="B171" s="2">
-        <v>95</v>
-      </c>
+      <c r="A171" s="2"/>
+      <c r="B171" s="2"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="2">
-        <v>564</v>
-      </c>
-      <c r="B172" s="2">
-        <v>91.5</v>
-      </c>
+      <c r="A172" s="2"/>
+      <c r="B172" s="2"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" s="2">
-        <v>565</v>
-      </c>
-      <c r="B173" s="2">
-        <v>86.5</v>
-      </c>
+      <c r="A173" s="2"/>
+      <c r="B173" s="2"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="2">
-        <v>567</v>
-      </c>
-      <c r="B174" s="2">
-        <v>76</v>
-      </c>
+      <c r="A174" s="2"/>
+      <c r="B174" s="2"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="2">
-        <v>568</v>
-      </c>
-      <c r="B175" s="2">
-        <v>69.5</v>
-      </c>
+      <c r="A175" s="2"/>
+      <c r="B175" s="2"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" s="2">
-        <v>570</v>
-      </c>
-      <c r="B176" s="2">
-        <v>57</v>
-      </c>
+      <c r="A176" s="2"/>
+      <c r="B176" s="2"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="2">
-        <v>571</v>
-      </c>
-      <c r="B177" s="2">
-        <v>51</v>
-      </c>
+      <c r="A177" s="2"/>
+      <c r="B177" s="2"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" s="2">
-        <v>572</v>
-      </c>
-      <c r="B178" s="2">
-        <v>45</v>
-      </c>
+      <c r="A178" s="2"/>
+      <c r="B178" s="2"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" s="2">
-        <v>573</v>
-      </c>
-      <c r="B179" s="2">
-        <v>34.5</v>
-      </c>
+      <c r="A179" s="2"/>
+      <c r="B179" s="2"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" s="2">
-        <v>575</v>
-      </c>
-      <c r="B180" s="2">
-        <v>30.5</v>
-      </c>
+      <c r="A180" s="2"/>
+      <c r="B180" s="2"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" s="2">
-        <v>576</v>
-      </c>
-      <c r="B181" s="2">
-        <v>26</v>
-      </c>
+      <c r="A181" s="2"/>
+      <c r="B181" s="2"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182" s="2">
-        <v>577</v>
-      </c>
-      <c r="B182" s="2">
-        <v>22.5</v>
-      </c>
+      <c r="A182" s="2"/>
+      <c r="B182" s="2"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" s="2">
-        <v>578</v>
-      </c>
-      <c r="B183" s="2">
-        <v>16.5</v>
-      </c>
+      <c r="A183" s="2"/>
+      <c r="B183" s="2"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" s="2">
-        <v>580</v>
-      </c>
-      <c r="B184" s="2">
-        <v>14</v>
-      </c>
+      <c r="A184" s="2"/>
+      <c r="B184" s="2"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="2">
-        <v>581</v>
-      </c>
-      <c r="B185" s="2">
-        <v>11.5</v>
-      </c>
+      <c r="A185" s="2"/>
+      <c r="B185" s="2"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" s="2">
-        <v>582</v>
-      </c>
-      <c r="B186" s="2">
-        <v>10</v>
-      </c>
+      <c r="A186" s="2"/>
+      <c r="B186" s="2"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" s="2">
-        <v>583</v>
-      </c>
-      <c r="B187" s="2">
-        <v>7</v>
-      </c>
+      <c r="A187" s="2"/>
+      <c r="B187" s="2"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" s="2">
-        <v>585</v>
-      </c>
-      <c r="B188" s="2">
-        <v>5.5</v>
-      </c>
+      <c r="A188" s="2"/>
+      <c r="B188" s="2"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" s="2">
-        <v>586</v>
-      </c>
-      <c r="B189" s="2">
-        <v>5</v>
-      </c>
+      <c r="A189" s="2"/>
+      <c r="B189" s="2"/>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="2">
-        <v>587</v>
-      </c>
-      <c r="B190" s="2">
-        <v>4</v>
-      </c>
+      <c r="A190" s="2"/>
+      <c r="B190" s="2"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" s="2">
-        <v>588</v>
-      </c>
-      <c r="B191" s="2">
-        <v>3</v>
-      </c>
+      <c r="A191" s="2"/>
+      <c r="B191" s="2"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" s="2">
-        <v>590</v>
-      </c>
-      <c r="B192" s="2">
-        <v>2.5</v>
-      </c>
+      <c r="A192" s="2"/>
+      <c r="B192" s="2"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" s="2">
-        <v>591</v>
-      </c>
-      <c r="B193" s="2">
-        <v>2.5</v>
-      </c>
+      <c r="A193" s="2"/>
+      <c r="B193" s="2"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A194" s="2">
-        <v>592</v>
-      </c>
-      <c r="B194" s="2">
-        <v>2</v>
-      </c>
+      <c r="A194" s="2"/>
+      <c r="B194" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>